<commit_message>
Finalizar seção de referência e deixar o texto coerente com a mesma; Atualizar formatação das tabelas
</commit_message>
<xml_diff>
--- a/Tabelas/Tabelas.xlsx
+++ b/Tabelas/Tabelas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Giovanni\Desktop\Monografia-USP\Tabelas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81F75CD1-A80C-4FD3-BD73-908FA8ED99EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7B21A5F-0AED-404E-849F-5F659CB42C1E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{3A68BAB9-AAAB-447F-8DC7-7F04D125C60E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{3A68BAB9-AAAB-447F-8DC7-7F04D125C60E}"/>
   </bookViews>
   <sheets>
     <sheet name="Lista de Práticas" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="42">
   <si>
     <t>1. Checklist de Especificação de Requisitos</t>
   </si>
@@ -154,9 +154,6 @@
   </si>
   <si>
     <t>De 0 a 10, qual a chance de você utilizar estas técnicas em outros projetos?</t>
-  </si>
-  <si>
-    <t>Questionário de validação</t>
   </si>
   <si>
     <t>Questão</t>
@@ -169,7 +166,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -186,14 +183,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
@@ -204,6 +193,22 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -235,21 +240,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -294,6 +284,21 @@
         <color indexed="64"/>
       </right>
       <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -303,37 +308,33 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -652,8 +653,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0B6B80F-364B-40F4-A73C-E3C3E5FDAAB4}">
   <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -664,10 +665,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5"/>
+      <c r="B1" s="6"/>
     </row>
     <row r="2" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
@@ -686,10 +687,10 @@
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="5"/>
+      <c r="B4" s="6"/>
     </row>
     <row r="5" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
@@ -716,10 +717,10 @@
       </c>
     </row>
     <row r="8" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="5"/>
+      <c r="B8" s="6"/>
     </row>
     <row r="9" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
@@ -754,10 +755,10 @@
       </c>
     </row>
     <row r="13" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="5"/>
+      <c r="B13" s="6"/>
     </row>
     <row r="14" spans="1:2" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
@@ -792,10 +793,10 @@
       </c>
     </row>
     <row r="18" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="5"/>
+      <c r="B18" s="6"/>
     </row>
     <row r="19" spans="1:2" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
@@ -822,10 +823,10 @@
       </c>
     </row>
     <row r="22" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="4" t="s">
+      <c r="A22" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="5"/>
+      <c r="B22" s="6"/>
     </row>
     <row r="23" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
@@ -867,128 +868,119 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56E1495F-0250-4287-A786-A2A814ACDDFE}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.85546875" customWidth="1"/>
-    <col min="2" max="2" width="81.85546875" customWidth="1"/>
+    <col min="2" max="2" width="77" customWidth="1"/>
     <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="7"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
-        <v>42</v>
+      <c r="C1" s="4"/>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="8">
+        <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="C2" s="6"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="10">
-        <v>1</v>
-      </c>
-      <c r="B3" s="11" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="10">
-        <f>$A3+1</f>
+    <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="8">
+        <f>$A2+1</f>
         <v>2</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B3" s="9" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="10">
-        <f t="shared" ref="A5:A12" si="0">$A4+1</f>
+    <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="8">
+        <f t="shared" ref="A4:A11" si="0">$A3+1</f>
         <v>3</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B4" s="9" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="10">
+    <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="8">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B5" s="9" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="10">
+    <row r="6" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="8">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B6" s="9" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="10">
+    <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="8">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B7" s="9" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="10">
+    <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="8">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B8" s="9" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="10">
+    <row r="9" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="8">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B9" s="9" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="10">
+    <row r="10" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="8">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B10" s="9" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="10">
+    <row r="11" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="8">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B11" s="9" t="s">
         <v>39</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:B1"/>
-  </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adicionar: Seção de pesquisa; Preenchimento do Checklist; Refatoração simples na monografia
</commit_message>
<xml_diff>
--- a/Tabelas/Tabelas.xlsx
+++ b/Tabelas/Tabelas.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Giovanni\Desktop\Monografia-USP\Tabelas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7B21A5F-0AED-404E-849F-5F659CB42C1E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{763702B3-C562-44C1-BC70-F7A517A647EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{3A68BAB9-AAAB-447F-8DC7-7F04D125C60E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{3A68BAB9-AAAB-447F-8DC7-7F04D125C60E}"/>
   </bookViews>
   <sheets>
     <sheet name="Lista de Práticas" sheetId="1" r:id="rId1"/>
-    <sheet name="Questionário" sheetId="2" r:id="rId2"/>
+    <sheet name="Listar" sheetId="3" r:id="rId2"/>
+    <sheet name="Det. Intra" sheetId="4" r:id="rId3"/>
+    <sheet name="Det. Inter" sheetId="5" r:id="rId4"/>
+    <sheet name="Questionário" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,10 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="42">
-  <si>
-    <t>1. Checklist de Especificação de Requisitos</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="51">
   <si>
     <t>1.1 Identificador do Requisito / História</t>
   </si>
@@ -160,6 +160,36 @@
   </si>
   <si>
     <t>#</t>
+  </si>
+  <si>
+    <t>BDD-SC-001</t>
+  </si>
+  <si>
+    <t>Listar comprovantes de acordo com agência, conta e período.</t>
+  </si>
+  <si>
+    <t>[nome e e-mail serão preservados]</t>
+  </si>
+  <si>
+    <t>Portal Corporativo</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>BDD-SC-002</t>
+  </si>
+  <si>
+    <t>BDD-SC-003</t>
+  </si>
+  <si>
+    <t>1. Práticas para Especificação de Requisitos</t>
+  </si>
+  <si>
+    <t>Detalhar comprovante de Transferência Intrabancária.</t>
+  </si>
+  <si>
+    <t>Detalhar comprovante de Transferência Interbancária.</t>
   </si>
 </sst>
 </file>
@@ -322,12 +352,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -335,6 +359,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -653,8 +683,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0B6B80F-364B-40F4-A73C-E3C3E5FDAAB4}">
   <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -665,191 +695,191 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="6"/>
+      <c r="A1" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="9"/>
     </row>
     <row r="2" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="6"/>
+      <c r="B4" s="9"/>
     </row>
     <row r="5" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="6"/>
+      <c r="A8" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="9"/>
     </row>
     <row r="9" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" s="6"/>
+      <c r="A13" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="9"/>
     </row>
     <row r="14" spans="1:2" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18" s="6"/>
+      <c r="A18" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="9"/>
     </row>
     <row r="19" spans="1:2" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B22" s="6"/>
+      <c r="B22" s="9"/>
     </row>
     <row r="23" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -867,10 +897,658 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FA5D4BA-FAFB-4796-9E5A-208C804640A9}">
+  <dimension ref="A1:B25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="36" style="1" customWidth="1"/>
+    <col min="2" max="2" width="44" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="9"/>
+    </row>
+    <row r="2" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="9"/>
+    </row>
+    <row r="5" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="9"/>
+    </row>
+    <row r="9" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="9"/>
+    </row>
+    <row r="14" spans="1:2" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="9"/>
+    </row>
+    <row r="19" spans="1:2" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" s="9"/>
+    </row>
+    <row r="23" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A22:B22"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60DFA4E8-0B84-436D-87E7-09C7118A4C5C}">
+  <dimension ref="A1:B25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="36" style="1" customWidth="1"/>
+    <col min="2" max="2" width="44" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="9"/>
+    </row>
+    <row r="2" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="9"/>
+    </row>
+    <row r="5" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="9"/>
+    </row>
+    <row r="9" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="9"/>
+    </row>
+    <row r="14" spans="1:2" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="9"/>
+    </row>
+    <row r="19" spans="1:2" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" s="9"/>
+    </row>
+    <row r="23" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A22:B22"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48C67FC6-D602-476E-8E24-20ADFA510ACB}">
+  <dimension ref="A1:B25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="36" style="1" customWidth="1"/>
+    <col min="2" max="2" width="44" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="9"/>
+    </row>
+    <row r="2" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="9"/>
+    </row>
+    <row r="5" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="9"/>
+    </row>
+    <row r="9" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="9"/>
+    </row>
+    <row r="14" spans="1:2" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="9"/>
+    </row>
+    <row r="19" spans="1:2" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" s="9"/>
+    </row>
+    <row r="23" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A22:B22"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56E1495F-0250-4287-A786-A2A814ACDDFE}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -882,101 +1560,101 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="B1" s="7" t="s">
+      <c r="A1" s="5" t="s">
         <v>40</v>
       </c>
+      <c r="B1" s="5" t="s">
+        <v>39</v>
+      </c>
       <c r="C1" s="4"/>
     </row>
     <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="8">
+      <c r="A2" s="6">
         <v>1</v>
       </c>
-      <c r="B2" s="9" t="s">
-        <v>30</v>
+      <c r="B2" s="7" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="8">
+      <c r="A3" s="6">
         <f>$A2+1</f>
         <v>2</v>
       </c>
-      <c r="B3" s="9" t="s">
-        <v>31</v>
+      <c r="B3" s="7" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="8">
+      <c r="A4" s="6">
         <f t="shared" ref="A4:A11" si="0">$A3+1</f>
         <v>3</v>
       </c>
-      <c r="B4" s="9" t="s">
-        <v>32</v>
+      <c r="B4" s="7" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="8">
+      <c r="A5" s="6">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B5" s="9" t="s">
-        <v>33</v>
+      <c r="B5" s="7" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="8">
+      <c r="A6" s="6">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B6" s="9" t="s">
-        <v>34</v>
+      <c r="B6" s="7" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="8">
+      <c r="A7" s="6">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B7" s="9" t="s">
-        <v>35</v>
+      <c r="B7" s="7" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="8">
+      <c r="A8" s="6">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B8" s="9" t="s">
-        <v>36</v>
+      <c r="B8" s="7" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="8">
+      <c r="A9" s="6">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B9" s="9" t="s">
-        <v>37</v>
+      <c r="B9" s="7" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="8">
+      <c r="A10" s="6">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B10" s="9" t="s">
-        <v>38</v>
+      <c r="B10" s="7" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="8">
+      <c r="A11" s="6">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B11" s="9" t="s">
-        <v>39</v>
+      <c r="B11" s="7" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refatoração inicial para qualificação
</commit_message>
<xml_diff>
--- a/Tabelas/Tabelas.xlsx
+++ b/Tabelas/Tabelas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Giovanni\Desktop\Monografia-USP\Tabelas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{763702B3-C562-44C1-BC70-F7A517A647EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1897BF08-6634-4158-A5EA-91B5087392D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{3A68BAB9-AAAB-447F-8DC7-7F04D125C60E}"/>
+    <workbookView xWindow="-19320" yWindow="-2340" windowWidth="19440" windowHeight="15000" xr2:uid="{3A68BAB9-AAAB-447F-8DC7-7F04D125C60E}"/>
   </bookViews>
   <sheets>
     <sheet name="Lista de Práticas" sheetId="1" r:id="rId1"/>
@@ -57,9 +57,6 @@
     <t>2.3 Desenvolvedor</t>
   </si>
   <si>
-    <t>3.1 Domínio do sistema mantido pelo time envolvido</t>
-  </si>
-  <si>
     <t>3.2 PO ou Representante de Negócio</t>
   </si>
   <si>
@@ -190,6 +187,9 @@
   </si>
   <si>
     <t>Detalhar comprovante de Transferência Interbancária.</t>
+  </si>
+  <si>
+    <t>3.1 Domínio do sistema mantido pela equipe envolvida</t>
   </si>
 </sst>
 </file>
@@ -684,7 +684,7 @@
   <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -696,7 +696,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B1" s="9"/>
     </row>
@@ -705,7 +705,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -713,7 +713,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -727,7 +727,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -735,7 +735,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -743,143 +743,143 @@
         <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8" s="9"/>
     </row>
     <row r="9" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B13" s="9"/>
     </row>
     <row r="14" spans="1:2" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B18" s="9"/>
     </row>
     <row r="19" spans="1:2" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B22" s="9"/>
     </row>
     <row r="23" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B24" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -901,7 +901,7 @@
   <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -913,7 +913,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B1" s="9"/>
     </row>
@@ -922,7 +922,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -930,7 +930,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -944,7 +944,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -952,7 +952,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -960,153 +960,153 @@
         <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8" s="9"/>
     </row>
     <row r="9" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B13" s="9"/>
     </row>
     <row r="14" spans="1:2" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B18" s="9"/>
     </row>
     <row r="19" spans="1:2" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B22" s="9"/>
     </row>
     <row r="23" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A22:B22"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A22:B22"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -1117,7 +1117,7 @@
   <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:B4"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1129,7 +1129,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B1" s="9"/>
     </row>
@@ -1138,7 +1138,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -1146,7 +1146,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1160,7 +1160,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1168,7 +1168,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1176,153 +1176,153 @@
         <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8" s="9"/>
     </row>
     <row r="9" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B13" s="9"/>
     </row>
     <row r="14" spans="1:2" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B18" s="9"/>
     </row>
     <row r="19" spans="1:2" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B22" s="9"/>
     </row>
     <row r="23" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A22:B22"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A22:B22"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -1333,7 +1333,7 @@
   <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:B4"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1345,7 +1345,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B1" s="9"/>
     </row>
@@ -1354,7 +1354,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -1362,7 +1362,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1376,7 +1376,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1384,7 +1384,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1392,153 +1392,153 @@
         <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8" s="9"/>
     </row>
     <row r="9" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B13" s="9"/>
     </row>
     <row r="14" spans="1:2" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B18" s="9"/>
     </row>
     <row r="19" spans="1:2" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B22" s="9"/>
     </row>
     <row r="23" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A22:B22"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A22:B22"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -1561,10 +1561,10 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C1" s="4"/>
     </row>
@@ -1573,7 +1573,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1582,7 +1582,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1591,7 +1591,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1600,7 +1600,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -1609,7 +1609,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1618,7 +1618,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1627,7 +1627,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -1636,7 +1636,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -1645,7 +1645,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1654,7 +1654,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactor Cap 3 e 4
</commit_message>
<xml_diff>
--- a/Tabelas/Tabelas.xlsx
+++ b/Tabelas/Tabelas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Giovanni\Desktop\Monografia-USP\Tabelas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1897BF08-6634-4158-A5EA-91B5087392D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D1EEC92-4FAD-4E89-BC20-C2C5C75A2483}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="-2340" windowWidth="19440" windowHeight="15000" xr2:uid="{3A68BAB9-AAAB-447F-8DC7-7F04D125C60E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5" xr2:uid="{3A68BAB9-AAAB-447F-8DC7-7F04D125C60E}"/>
   </bookViews>
   <sheets>
     <sheet name="Lista de Práticas" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Det. Intra" sheetId="4" r:id="rId3"/>
     <sheet name="Det. Inter" sheetId="5" r:id="rId4"/>
     <sheet name="Questionário" sheetId="2" r:id="rId5"/>
+    <sheet name="Questões Dissertativas" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="67">
   <si>
     <t>1.1 Identificador do Requisito / História</t>
   </si>
@@ -190,13 +191,61 @@
   </si>
   <si>
     <t>3.1 Domínio do sistema mantido pela equipe envolvida</t>
+  </si>
+  <si>
+    <t>Entendimento claro do que fazer e de quem procurar em caso de dúvidas ou problemas, apesar de praticamente não ter existido essa necessidade.</t>
+  </si>
+  <si>
+    <t>Praticamente não houve retrabalho, tínhamos o contato de todos e sabíamos com quem tirar dúvidas e aonde estava a documentação</t>
+  </si>
+  <si>
+    <t>Só começamos a desenvolver depois de fechar o requisito</t>
+  </si>
+  <si>
+    <t>O entendimento ficou claro devido as conversas que tivemos e a padronização dos documentos</t>
+  </si>
+  <si>
+    <t>Preocupação em validar se todos sabiam o que precisava fazer e a lista de contatos deu uma boa base para as comunicações.</t>
+  </si>
+  <si>
+    <t>maior foco em entender a necessidade do projeto</t>
+  </si>
+  <si>
+    <t>A participação de todos no momento de modelar, os problemas no entendimento foram detectados em momentos iniciais, diante disso houve menos retrabalho.</t>
+  </si>
+  <si>
+    <t>Validações do escopo com todos os envolvidos e início do desenvolvimento após formalização de entendimento .</t>
+  </si>
+  <si>
+    <t>Não, a comunicação é essencial para qualquer projeto ou entrega de feature.</t>
+  </si>
+  <si>
+    <t>Não, a comunicação aliada a uma boa modelagem faz toda a diferença para um entrega bem sucedida e com o mínimo de retrabalho</t>
+  </si>
+  <si>
+    <t>Não</t>
+  </si>
+  <si>
+    <t>Não, sempre haverá dúvidas e/ou pontos a serem discutidos, então uma gestão de comunicação é necessária.</t>
+  </si>
+  <si>
+    <t>Nao, sem uma boa gestão de comunicação as informações acabam se perdendo durante o desenvolvimento do projeto.</t>
+  </si>
+  <si>
+    <t>uma boa comunicação é essencial sim para uma boa entrega</t>
+  </si>
+  <si>
+    <t>Não, pois se nem todos estiverem atualizados sobre o que foi definido ainda teremos problemas de entendimento</t>
+  </si>
+  <si>
+    <t>A modelagem de requisitos bem feita, facilita demais na entrega de um projeto, mas sem a gestão de comunicações, os blocks e retrabalhos se tornam presentes, pois fazem com que os riscos não sejam compartilhados de forma rápida e eficiente.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -239,6 +288,10 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="4">
@@ -335,10 +388,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -367,9 +421,22 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{6AF60117-198B-4719-AB64-9C1267EEB17E}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -683,8 +750,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0B6B80F-364B-40F4-A73C-E3C3E5FDAAB4}">
   <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1549,7 +1616,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1661,4 +1728,153 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43965682-18FC-4492-9B9C-49A11CBE32FF}">
+  <dimension ref="A1:B19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="36" style="1" customWidth="1"/>
+    <col min="2" max="2" width="44" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="11"/>
+    </row>
+    <row r="2" spans="1:2" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="12"/>
+    </row>
+    <row r="3" spans="1:2" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" s="12"/>
+    </row>
+    <row r="4" spans="1:2" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" s="12"/>
+    </row>
+    <row r="5" spans="1:2" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" s="12"/>
+    </row>
+    <row r="6" spans="1:2" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6" s="12"/>
+    </row>
+    <row r="7" spans="1:2" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" s="12"/>
+    </row>
+    <row r="8" spans="1:2" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8" s="12"/>
+    </row>
+    <row r="9" spans="1:2" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="B9" s="12"/>
+    </row>
+    <row r="10" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:2" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="11"/>
+    </row>
+    <row r="12" spans="1:2" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="B12" s="12"/>
+    </row>
+    <row r="13" spans="1:2" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="B13" s="12"/>
+    </row>
+    <row r="14" spans="1:2" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="B14" s="12"/>
+    </row>
+    <row r="15" spans="1:2" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="B15" s="12"/>
+    </row>
+    <row r="16" spans="1:2" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="B16" s="12"/>
+    </row>
+    <row r="17" spans="1:2" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="B17" s="12"/>
+    </row>
+    <row r="18" spans="1:2" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="B18" s="12"/>
+    </row>
+    <row r="19" spans="1:2" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="B19" s="12"/>
+    </row>
+  </sheetData>
+  <mergeCells count="18">
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>